<commit_message>
Fix reference to non-existing model
</commit_message>
<xml_diff>
--- a/Tables/Unmappable_RNA-seq_genes.xlsx
+++ b/Tables/Unmappable_RNA-seq_genes.xlsx
@@ -25,12 +25,12 @@
     <t>Name</t>
   </si>
   <si>
+    <t>645740.1</t>
+  </si>
+  <si>
     <t>201288.1</t>
   </si>
   <si>
-    <t>645740.1</t>
-  </si>
-  <si>
     <t>728441.1</t>
   </si>
   <si>
@@ -55,30 +55,30 @@
     <t>8041.1</t>
   </si>
   <si>
+    <t>340811.1</t>
+  </si>
+  <si>
     <t>100288072.1</t>
   </si>
   <si>
-    <t>340811.1</t>
-  </si>
-  <si>
     <t>0</t>
   </si>
   <si>
     <t>4514.1</t>
   </si>
   <si>
+    <t>4512.1</t>
+  </si>
+  <si>
     <t>4513.1</t>
   </si>
   <si>
-    <t>4512.1</t>
+    <t>NOS2P1</t>
   </si>
   <si>
     <t>NOS2P2</t>
   </si>
   <si>
-    <t>NOS2P1</t>
-  </si>
-  <si>
     <t>GGT2</t>
   </si>
   <si>
@@ -97,27 +97,27 @@
     <t>HEXD</t>
   </si>
   <si>
+    <t>AKR1C8P</t>
+  </si>
+  <si>
     <t>SDR42E2</t>
   </si>
   <si>
-    <t>AKR1C8P</t>
-  </si>
-  <si>
     <t>COX3</t>
   </si>
   <si>
+    <t>COX1</t>
+  </si>
+  <si>
     <t>COX2</t>
   </si>
   <si>
-    <t>COX1</t>
+    <t>NOS2C</t>
   </si>
   <si>
     <t>NOS2B</t>
   </si>
   <si>
-    <t>NOS2C</t>
-  </si>
-  <si>
     <t>['GGT', 'GGT 2']</t>
   </si>
   <si>
@@ -142,18 +142,18 @@
     <t>['COIII', 'MTCO3']</t>
   </si>
   <si>
+    <t>['COI', 'MTCO1']</t>
+  </si>
+  <si>
     <t>['COII', 'MTCO2']</t>
   </si>
   <si>
-    <t>['COI', 'MTCO1']</t>
+    <t>nitric oxide synthase 2 pseudogene 1</t>
   </si>
   <si>
     <t>nitric oxide synthase 2 pseudogene 2</t>
   </si>
   <si>
-    <t>nitric oxide synthase 2 pseudogene 1</t>
-  </si>
-  <si>
     <t>gamma-glutamyltransferase 2</t>
   </si>
   <si>
@@ -172,19 +172,19 @@
     <t>hexosaminidase D</t>
   </si>
   <si>
+    <t>aldo-keto reductase family 1 member C8, pseudogene</t>
+  </si>
+  <si>
     <t>short chain dehydrogenase/reductase family 42E, member 2</t>
   </si>
   <si>
-    <t>aldo-keto reductase family 1 member C8, pseudogene</t>
-  </si>
-  <si>
     <t>cytochrome c oxidase III</t>
   </si>
   <si>
+    <t>cytochrome c oxidase subunit I</t>
+  </si>
+  <si>
     <t>cytochrome c oxidase subunit II</t>
-  </si>
-  <si>
-    <t>cytochrome c oxidase subunit I</t>
   </si>
 </sst>
 </file>
@@ -688,6 +688,9 @@
       <c r="B12" t="s">
         <v>27</v>
       </c>
+      <c r="C12" t="s">
+        <v>40</v>
+      </c>
       <c r="D12" t="s">
         <v>52</v>
       </c>
@@ -698,9 +701,6 @@
       </c>
       <c r="B13" t="s">
         <v>28</v>
-      </c>
-      <c r="C13" t="s">
-        <v>40</v>
       </c>
       <c r="D13" t="s">
         <v>53</v>

</xml_diff>